<commit_message>
new update to have an alternative to be more safety conscious rule.
</commit_message>
<xml_diff>
--- a/TR2MTL_Traffic Rule Evaluation Dataset.xlsx
+++ b/TR2MTL_Traffic Rule Evaluation Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\TR2MTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9FE12D-FFD7-4B6B-B1C5-E17E76E7F61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C088E52-4A6E-473B-857C-DB89ECFC9818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
   <si>
     <t>Traffic rule</t>
   </si>
@@ -261,20 +261,10 @@
     </r>
   </si>
   <si>
-    <t>G(at_intersection(ego) &amp; ~traffic_sign(ego,stop) &amp; ~traffic_sign(ego,yield) -&gt;
-  (P[0,t]in_intersection(traffic) -&gt;
-  yield(ego,other)))</t>
-  </si>
-  <si>
     <t>DMV:page 47 (intersection)</t>
   </si>
   <si>
     <t>At intersections without stop or yield signs, yield to the vehicle on your right if it reaches the intersection at the same time as you.</t>
-  </si>
-  <si>
-    <t>G(at_intersection(ego) &amp; at_intersection(other) ~traffic_sign(ego,stop) &amp; ~traffic_sign(ego,yield) -&gt;
-  (P[0,t]in_intersection(traffic) -&gt;
-  yield(ego,other)))"</t>
   </si>
   <si>
     <t>During overtaking, a sufficient lateral distance must be kept from other road users, particularly pedestrians and pedal cyclists.</t>
@@ -343,20 +333,40 @@
     <t>G((at_intersection(ego) | at_junction(ego)) &amp; right_of(other,ego)-&gt; yield(ego,other))</t>
   </si>
   <si>
-    <t>same as safe distance rule mentioned above, only ist for pedestrian and earlier it was just denoted with other</t>
-  </si>
-  <si>
     <t>Ego must stop behind the line at a junction with a Stop sign and a solid white line across the road. Wait for a safe gap in the traffic before you move off."</t>
   </si>
   <si>
-    <t>at(ego, junction) &amp; at_traffic_sign(junction,stop) -&gt; stop(ego) U safe_distance(ego, other)</t>
+    <t>same as safe distance rule mentioned above, only it is for pedestrian and earlier it was just denoted with other</t>
+  </si>
+  <si>
+    <t>G(at_intersection(ego) &amp; ~traffic_sign(ego,stop) &amp; ~traffic_sign(ego,yield) -&gt;
+  (P[0,t]in_intersection(traffic) -&gt; yield(ego,other)))</t>
+  </si>
+  <si>
+    <t>G(at_intersection(ego) &amp; at_intersection(other) ~traffic_sign(ego,stop) &amp; ~traffic_sign(ego,yield) -&gt;
+  (P[0,t]in_intersection(traffic) -&gt;yield(ego,other)))</t>
+  </si>
+  <si>
+    <t>at(ego, junction) &amp; at_traffic_sign(ego,stop) -&gt; stop(ego) U safe_distance(ego, other)</t>
+  </si>
+  <si>
+    <t>Note we can add restrictions over in how many times maximum they have to procees or stop</t>
+  </si>
+  <si>
+    <t>G((at_intersection(ego) &amp; traffic_light(ego,red) -&gt;F[0,2](stop(ego))) ∧ (traffic_light(ego,green) -&gt; F[0,2](proceed(ego))))</t>
+  </si>
+  <si>
+    <t>At intersections with traffic lights, drivers must stop at a red light within 3 seconds and may proceed at a green light within 3 seconds.</t>
+  </si>
+  <si>
+    <t>same rule but with more safety property</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -404,6 +414,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -425,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -443,6 +460,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,17 +682,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1003"/>
+  <dimension ref="A1:D1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="88.6640625" customWidth="1"/>
     <col min="2" max="2" width="100.44140625" customWidth="1"/>
-    <col min="3" max="3" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="52.109375" customWidth="1"/>
     <col min="4" max="4" width="42.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -842,7 +863,7 @@
         <v>41</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -867,7 +888,7 @@
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -886,7 +907,7 @@
         <v>49</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>30</v>
@@ -894,7 +915,7 @@
     </row>
     <row r="22" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>52</v>
@@ -908,7 +929,7 @@
         <v>54</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>30</v>
@@ -945,149 +966,162 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="C33" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="B34" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="C34" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
     </row>
@@ -4911,8 +4945,13 @@
       <c r="A1003" s="2"/>
       <c r="B1003" s="2"/>
     </row>
+    <row r="1004" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1004" s="2"/>
+      <c r="B1004" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;8&amp;K000000 Internal</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
deleted extra changed row
</commit_message>
<xml_diff>
--- a/TR2MTL_Traffic Rule Evaluation Dataset.xlsx
+++ b/TR2MTL_Traffic Rule Evaluation Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\TR2MTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C088E52-4A6E-473B-857C-DB89ECFC9818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1E2598-E30F-42F3-97A8-A2ADB6A270B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>Traffic rule</t>
   </si>
@@ -131,12 +131,6 @@
   </si>
   <si>
     <t>VCoRT: article. 11(2)(a)</t>
-  </si>
-  <si>
-    <t>on the special driveway only prescribed vehicle are allowed to pass and if ego is not prescribed Vehicle it should not travel om special driveway.</t>
-  </si>
-  <si>
-    <t>G(only_prescribed_vehicles_on_special_driveway &amp; (~ego_prescribed_vehicle -&gt; ~travel_on_special_driveway(ego)))</t>
   </si>
   <si>
     <t>It is always the case that if the other vehicle is to the left of the ego vehicle and the ego vehicle drives faster than the other vehicle, then the ego vehicle is to the right of a broad lane marking and the other vehicle is to the left of a solid lane marking.</t>
@@ -682,10 +676,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D1004"/>
+  <dimension ref="A1:D1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -833,10 +827,10 @@
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>30</v>
@@ -850,90 +844,91 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>44</v>
       </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
       <c r="B18" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="B19" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="2" t="s">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="B23" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -942,58 +937,60 @@
       <c r="B24" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C24" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="7" t="s">
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="B29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
@@ -1001,81 +998,74 @@
         <v>63</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="A33" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" s="10" t="s">
         <v>74</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>77</v>
-      </c>
+    </row>
+    <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="2" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="37" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
@@ -4944,10 +4934,6 @@
     <row r="1003" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1003" s="2"/>
       <c r="B1003" s="2"/>
-    </row>
-    <row r="1004" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1004" s="2"/>
-      <c r="B1004" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removal of additional created rule
</commit_message>
<xml_diff>
--- a/TR2MTL_Traffic Rule Evaluation Dataset.xlsx
+++ b/TR2MTL_Traffic Rule Evaluation Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\TR2MTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1E2598-E30F-42F3-97A8-A2ADB6A270B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B62E557-1EE4-4AFB-B075-C4EB3797736E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>ego shall not overtake another vehicle if a pedestrian crosswalk is in front of the other vehicle.</t>
-  </si>
-  <si>
-    <t>G(~overtake(ego, other_vehicle) -&gt; in_front_of(other_vehicle,crosswalk))</t>
   </si>
   <si>
     <t>VCoRT:Article 11.9</t>
@@ -354,6 +351,9 @@
   </si>
   <si>
     <t>same rule but with more safety property</t>
+  </si>
+  <si>
+    <t>G(~overtake(ego, other_vehicle) -&gt; in_front_of(crosswalk,other_vehicle))</t>
   </si>
 </sst>
 </file>
@@ -678,8 +678,8 @@
   </sheetPr>
   <dimension ref="A1:D1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -709,358 +709,358 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" t="s">
         <v>89</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed file info and structure.
</commit_message>
<xml_diff>
--- a/TR2MTL_Traffic Rule Evaluation Dataset.xlsx
+++ b/TR2MTL_Traffic Rule Evaluation Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\TR2MTL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B62E557-1EE4-4AFB-B075-C4EB3797736E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CA3537-C587-4241-A39D-982DBFC2B6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>If the ego vehicle is not part of congestion or if the directly leading vehicle is not standing, then stopping on the main carriage way, shoulder lane, or ramps is forbidden.</t>
-  </si>
-  <si>
-    <t>G(~congestion(ego) &amp; (~standing(leading) -&gt; ~(stop_main_carriageway(ego) | stop_shoulder_lane(ego) | stop_ramps(ego))))</t>
   </si>
   <si>
     <t>StVO: § 18 Rn. 22, § 12(1), § 18(8)</t>
@@ -354,6 +351,9 @@
   </si>
   <si>
     <t>G(~overtake(ego, other_vehicle) -&gt; in_front_of(crosswalk,other_vehicle))</t>
+  </si>
+  <si>
+    <t>G(~congestion(ego) |  (~standing(leading) -&gt; ~(stop_main_carriageway(ego) | stop_shoulder_lane(ego) | stop_ramps(ego))))</t>
   </si>
 </sst>
 </file>
@@ -679,7 +679,7 @@
   <dimension ref="A1:D1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -750,317 +750,317 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" t="s">
         <v>88</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>